<commit_message>
modify testcase template:add all iterations
</commit_message>
<xml_diff>
--- a/doc/Testcases.xlsx
+++ b/doc/Testcases.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-300" yWindow="460" windowWidth="38400" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="3" r:id="rId1"/>
     <sheet name="Iteration1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Iteration2" sheetId="5" r:id="rId3"/>
+    <sheet name="Iteration3" sheetId="6" r:id="rId4"/>
+    <sheet name="Iteration4" sheetId="7" r:id="rId5"/>
+    <sheet name="Iteration5" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="28">
   <si>
     <t>Schedule</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -130,9 +133,6 @@
   </si>
   <si>
     <t>user can see list of receipt information</t>
-  </si>
-  <si>
-    <t>2008-08-102016-05-26</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -645,77 +645,89 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1027,7 @@
       </c>
       <c r="B1" s="22">
         <f ca="1">TODAY()</f>
-        <v>42516</v>
+        <v>42517</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1026,91 +1038,91 @@
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="29"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>1</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="33"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>2</v>
       </c>
       <c r="B5" s="19"/>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>3</v>
       </c>
       <c r="B6" s="19"/>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25" t="s">
+      <c r="D6" s="32"/>
+      <c r="E6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>4</v>
       </c>
       <c r="B7" s="19"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="27"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>5</v>
       </c>
       <c r="B8" s="19"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="27"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1121,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,65 +1145,61 @@
   <sheetData>
     <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="29"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="28" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42" t="s">
+      <c r="F5" s="43"/>
+      <c r="G5" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="29"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45">
-        <v>39671</v>
-      </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="43">
-        <v>39673</v>
-      </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="45">
-        <v>39673</v>
-      </c>
-      <c r="H6" s="46"/>
+      <c r="A6" s="38">
+        <v>42531</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40">
+        <v>42533</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="29"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1212,10 +1220,10 @@
       <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="29"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
@@ -1228,7 +1236,7 @@
       </c>
       <c r="C10" s="8">
         <f>COUNTIF(I14:I42,"Pass")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="8">
         <f>COUNTIF(I14:I42,"Fail")</f>
@@ -1240,13 +1248,13 @@
       </c>
       <c r="F10" s="10">
         <f>C10/B10</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="G10" s="39" t="e">
+        <v>1</v>
+      </c>
+      <c r="G10" s="46" t="e">
         <f>E10/D10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H10" s="40"/>
+      <c r="H10" s="47"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1257,18 +1265,18 @@
       <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="28" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="34" t="s">
+      <c r="F13" s="28"/>
+      <c r="G13" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="35"/>
+      <c r="H13" s="49"/>
       <c r="I13" s="12" t="s">
         <v>17</v>
       </c>
@@ -1281,16 +1289,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="15"/>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32" t="s">
+      <c r="D14" s="30"/>
+      <c r="E14" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="31"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="30"/>
       <c r="I14" s="16" t="s">
         <v>19</v>
       </c>
@@ -1301,16 +1309,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="19"/>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25" t="s">
+      <c r="D15" s="32"/>
+      <c r="E15" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="26"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="20" t="s">
         <v>19</v>
       </c>
@@ -1321,16 +1329,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="19"/>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25" t="s">
+      <c r="D16" s="32"/>
+      <c r="E16" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="26"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="20" t="s">
         <v>19</v>
       </c>
@@ -1341,15 +1349,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="20" t="s">
-        <v>19</v>
-      </c>
+      <c r="C17" s="35"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="20"/>
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1357,19 +1363,38 @@
         <v>5</v>
       </c>
       <c r="B18" s="19"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="20" t="s">
-        <v>19</v>
-      </c>
+      <c r="C18" s="35"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="20"/>
       <c r="J18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
@@ -1379,27 +1404,6 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I14:I18">
@@ -1416,12 +1420,1156 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" zoomScale="119" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="6" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>42545</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40">
+        <v>42547</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <f>COUNTA(C14:D42)</f>
+        <v>3</v>
+      </c>
+      <c r="B10" s="7">
+        <f>A10-COUNTIF(I14:I42,"N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <f>COUNTIF(I14:I42,"Pass")</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <f>COUNTIF(I14:I42,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <f>COUNTIF(J14:J42,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <f>C10/B10</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="46" t="e">
+        <f>E10/D10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="49"/>
+      <c r="I13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="34"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>3</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>4</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14:J18">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I14:I18">
+      <formula1>"Pass,Fail,N/A"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:J18"/>
+  <sheetViews>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="6" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>42559</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40">
+        <v>42561</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <f>COUNTA(C14:D42)</f>
+        <v>3</v>
+      </c>
+      <c r="B10" s="7">
+        <f>A10-COUNTIF(I14:I42,"N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <f>COUNTIF(I14:I42,"Pass")</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <f>COUNTIF(I14:I42,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <f>COUNTIF(J14:J42,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <f>C10/B10</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="46" t="e">
+        <f>E10/D10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="49"/>
+      <c r="I13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="34"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>3</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>4</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I14:I18">
+      <formula1>"Pass,Fail,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14:J18">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:J18"/>
+  <sheetViews>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="6" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>42573</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40">
+        <v>42575</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <f>COUNTA(C14:D42)</f>
+        <v>3</v>
+      </c>
+      <c r="B10" s="7">
+        <f>A10-COUNTIF(I14:I42,"N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <f>COUNTIF(I14:I42,"Pass")</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <f>COUNTIF(I14:I42,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <f>COUNTIF(J14:J42,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <f>C10/B10</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="46" t="e">
+        <f>E10/D10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="49"/>
+      <c r="I13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="34"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>3</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>4</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14:J18">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I14:I18">
+      <formula1>"Pass,Fail,N/A"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:J18"/>
+  <sheetViews>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="6" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>42587</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40">
+        <v>42589</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <f>COUNTA(C14:D42)</f>
+        <v>3</v>
+      </c>
+      <c r="B10" s="7">
+        <f>A10-COUNTIF(I14:I42,"N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <f>COUNTIF(I14:I42,"Pass")</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <f>COUNTIF(I14:I42,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <f>COUNTIF(J14:J42,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <f>C10/B10</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="46" t="e">
+        <f>E10/D10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="49"/>
+      <c r="I13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="34"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>3</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>4</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I14:I18">
+      <formula1>"Pass,Fail,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14:J18">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>